<commit_message>
Test headers from CodeJava.com
</commit_message>
<xml_diff>
--- a/JavaBooks.xlsx
+++ b/JavaBooks.xlsx
@@ -12,7 +12,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
   <si>
     <t>Head First Java</t>
   </si>
@@ -43,13 +52,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <b val="true"/>
     </font>
   </fonts>
   <fills count="2">
@@ -72,26 +86,39 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="B2:D5"/>
+  <dimension ref="B1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
+    <row r="1">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="2">
       <c r="B2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D2" t="n">
         <v>79.0</v>
@@ -99,10 +126,10 @@
     </row>
     <row r="3">
       <c r="B3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D3" t="n">
         <v>36.0</v>
@@ -110,10 +137,10 @@
     </row>
     <row r="4">
       <c r="B4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D4" t="n">
         <v>42.0</v>
@@ -121,10 +148,10 @@
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D5" t="n">
         <v>35.0</v>

</xml_diff>

<commit_message>
Open file after creating xlsx
</commit_message>
<xml_diff>
--- a/JavaBooks.xlsx
+++ b/JavaBooks.xlsx
@@ -12,15 +12,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
-    <t>Title</t>
+    <t>Date</t>
   </si>
   <si>
-    <t>Author</t>
+    <t>Description</t>
   </si>
   <si>
-    <t>Price</t>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Amount</t>
   </si>
   <si>
     <t>Head First Java</t>
@@ -110,15 +113,15 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2">
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2" t="n">
         <v>79.0</v>
@@ -126,10 +129,10 @@
     </row>
     <row r="3">
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" t="n">
         <v>36.0</v>
@@ -137,10 +140,10 @@
     </row>
     <row r="4">
       <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" t="n">
         <v>42.0</v>
@@ -148,10 +151,10 @@
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5" t="n">
         <v>35.0</v>

</xml_diff>